<commit_message>
Fixed some bugs, check the QA Excel file
</commit_message>
<xml_diff>
--- a/COMPARC Project #2/QA Testing.xlsx
+++ b/COMPARC Project #2/QA Testing.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\markarevz18\Documents (D)\Github\COMPARC-Project\COMPARC Project #2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="23955" windowHeight="9780"/>
+    <workbookView xWindow="0" yWindow="132" windowWidth="23952" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>Condition</t>
   </si>
@@ -181,13 +186,22 @@
   </si>
   <si>
     <t>Fixed</t>
+  </si>
+  <si>
+    <t>This case is correct.</t>
+  </si>
+  <si>
+    <t>The actual format should not have a '#'</t>
+  </si>
+  <si>
+    <t>Many error messages but it doesn't crash anymore</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,22 +303,22 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -322,10 +336,10 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -343,18 +357,24 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G1048576" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G1048576">
-    <filterColumn colId="6"/>
-  </autoFilter>
+  <autoFilter ref="A1:G1048576"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Test Case" dataDxfId="6"/>
     <tableColumn id="2" name="Condition" dataDxfId="5"/>
@@ -411,7 +431,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -443,9 +463,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -477,6 +498,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -652,24 +674,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E40" sqref="A39:E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="39" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.85546875" style="1" customWidth="1"/>
-    <col min="6" max="7" width="43.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.88671875" style="1" customWidth="1"/>
+    <col min="6" max="7" width="43.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -702,7 +724,7 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -721,7 +743,7 @@
       </c>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -732,7 +754,7 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -753,7 +775,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>3</v>
       </c>
@@ -772,7 +794,7 @@
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -783,7 +805,7 @@
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -794,7 +816,7 @@
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>4</v>
       </c>
@@ -811,7 +833,7 @@
       </c>
       <c r="G11" s="3"/>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>5</v>
       </c>
@@ -830,7 +852,7 @@
       </c>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -841,7 +863,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>6</v>
       </c>
@@ -860,7 +882,7 @@
       </c>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -871,7 +893,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>7</v>
       </c>
@@ -890,7 +912,7 @@
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -901,11 +923,11 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E21"/>
       <c r="F21"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>8</v>
       </c>
@@ -924,7 +946,7 @@
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -935,10 +957,10 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>9</v>
       </c>
@@ -957,7 +979,7 @@
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -968,7 +990,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>10</v>
       </c>
@@ -980,12 +1002,12 @@
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="3" t="s">
-        <v>20</v>
+      <c r="F28" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
@@ -998,7 +1020,7 @@
       </c>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
@@ -1011,7 +1033,7 @@
       </c>
       <c r="G30" s="3"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>11</v>
       </c>
@@ -1028,7 +1050,7 @@
       </c>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4" t="s">
@@ -1041,7 +1063,7 @@
       </c>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
@@ -1054,7 +1076,7 @@
       </c>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4" t="s">
@@ -1067,7 +1089,7 @@
       </c>
       <c r="G35" s="4"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>12</v>
       </c>
@@ -1084,7 +1106,7 @@
       </c>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
@@ -1096,6 +1118,26 @@
         <v>53</v>
       </c>
       <c r="G38" s="3"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1107,24 +1149,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>